<commit_message>
Add flash message documentation
</commit_message>
<xml_diff>
--- a/vagrant/restaurantAppRoute.xlsx
+++ b/vagrant/restaurantAppRoute.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songseonghan/Documents/Autonomiq/FullStack/vagrant/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB521DD8-BF31-3F41-8F8A-FCC906358D59}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13BF844C-AC18-3148-91A8-E38BD3639051}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{4EFD2E4B-9604-ED40-879A-A5629E5AE994}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{4EFD2E4B-9604-ED40-879A-A5629E5AE994}"/>
   </bookViews>
   <sheets>
     <sheet name="Routing" sheetId="1" r:id="rId1"/>
     <sheet name="Template" sheetId="2" r:id="rId2"/>
     <sheet name="API " sheetId="3" r:id="rId3"/>
+    <sheet name="Flash_Msg" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="49">
   <si>
     <t>URL</t>
   </si>
@@ -163,6 +164,27 @@
   </si>
   <si>
     <t>menuItemJSON()</t>
+  </si>
+  <si>
+    <t>Flash_Message</t>
+  </si>
+  <si>
+    <t>New Restaurant Created</t>
+  </si>
+  <si>
+    <t>New MenuItem Created</t>
+  </si>
+  <si>
+    <t>Restaurant Successfully Edited</t>
+  </si>
+  <si>
+    <t>Menu Item successfully Edited</t>
+  </si>
+  <si>
+    <t>Restaurant Successfully Deleted</t>
+  </si>
+  <si>
+    <t>Menu Item successfully Deleted</t>
   </si>
 </sst>
 </file>
@@ -227,17 +249,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -577,132 +599,315 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="5" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="24">
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39088F18-0402-6748-BB33-A72F9C80BCFE}">
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="3" width="32.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="24">
@@ -735,195 +940,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39088F18-0402-6748-BB33-A72F9C80BCFE}">
-  <dimension ref="A1:C17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="3" width="32.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-    </row>
-  </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBB3AF68-0180-0946-B8F5-EC87985D0C84}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -967,4 +989,78 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{700777EA-F21F-344A-A7DC-825957F4812F}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="43.33203125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add styling using css file
</commit_message>
<xml_diff>
--- a/vagrant/restaurantAppRoute.xlsx
+++ b/vagrant/restaurantAppRoute.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songseonghan/Documents/Autonomiq/FullStack/vagrant/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13BF844C-AC18-3148-91A8-E38BD3639051}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CCF9B5B-7ABA-8746-977F-C5B0C556ACB2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{4EFD2E4B-9604-ED40-879A-A5629E5AE994}"/>
   </bookViews>
@@ -996,7 +996,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>